<commit_message>
新添加了ble bgt blt beqz bnez指令
</commit_message>
<xml_diff>
--- a/SingleCycle/truthtable.xlsx
+++ b/SingleCycle/truthtable.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="114">
   <si>
     <t>instruct</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -416,43 +416,63 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>0x03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010_110</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010_001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ori</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>beqz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bnez</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>J</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0x03</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>X</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>X</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>X</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>X</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>010_110</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>010_001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x0D</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ori</t>
+    <t>ble</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bgt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>blt</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -793,10 +813,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O32"/>
+  <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1159,7 +1179,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K8" s="2">
         <v>0</v>
@@ -1204,7 +1224,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K9" s="2">
         <v>0</v>
@@ -1812,10 +1832,10 @@
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>22</v>
@@ -2037,7 +2057,7 @@
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="1" t="s">
-        <v>74</v>
+        <v>111</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>85</v>
@@ -2082,7 +2102,7 @@
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="1" t="s">
-        <v>75</v>
+        <v>112</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>86</v>
@@ -2127,7 +2147,7 @@
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="1" t="s">
-        <v>76</v>
+        <v>113</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>87</v>
@@ -2170,20 +2190,18 @@
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>99</v>
-      </c>
+      <c r="A31" s="5"/>
       <c r="B31" s="1" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>34</v>
+        <v>83</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>101</v>
+        <v>22</v>
       </c>
       <c r="E31" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>22</v>
@@ -2191,14 +2209,14 @@
       <c r="G31" s="2">
         <v>0</v>
       </c>
-      <c r="H31" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>102</v>
+      <c r="H31" s="2">
+        <v>0</v>
+      </c>
+      <c r="I31" s="2">
+        <v>0</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>22</v>
+        <v>91</v>
       </c>
       <c r="K31" s="2">
         <v>0</v>
@@ -2206,66 +2224,293 @@
       <c r="L31" s="2">
         <v>0</v>
       </c>
-      <c r="M31" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N31" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="O31" s="2" t="s">
-        <v>58</v>
+      <c r="M31" t="s">
+        <v>22</v>
+      </c>
+      <c r="N31" s="2">
+        <v>1</v>
+      </c>
+      <c r="O31" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E32" s="2">
+        <v>1</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G32" s="2">
+        <v>0</v>
+      </c>
+      <c r="H32" s="2">
+        <v>0</v>
+      </c>
+      <c r="I32" s="2">
+        <v>0</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K32" s="2">
+        <v>0</v>
+      </c>
+      <c r="L32" s="2">
+        <v>0</v>
+      </c>
+      <c r="M32" t="s">
+        <v>22</v>
+      </c>
+      <c r="N32" s="2">
+        <v>1</v>
+      </c>
+      <c r="O32" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="5"/>
+      <c r="B33" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E33" s="2">
+        <v>1</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G33" s="2">
+        <v>0</v>
+      </c>
+      <c r="H33" s="2">
+        <v>0</v>
+      </c>
+      <c r="I33" s="2">
+        <v>0</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K33" s="2">
+        <v>0</v>
+      </c>
+      <c r="L33" s="2">
+        <v>0</v>
+      </c>
+      <c r="M33" t="s">
+        <v>22</v>
+      </c>
+      <c r="N33" s="2">
+        <v>1</v>
+      </c>
+      <c r="O33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="5"/>
+      <c r="B34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34" s="2">
+        <v>1</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G34" s="2">
+        <v>0</v>
+      </c>
+      <c r="H34" s="2">
+        <v>0</v>
+      </c>
+      <c r="I34" s="2">
+        <v>0</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K34" s="2">
+        <v>0</v>
+      </c>
+      <c r="L34" s="2">
+        <v>0</v>
+      </c>
+      <c r="M34" t="s">
+        <v>22</v>
+      </c>
+      <c r="N34" s="2">
+        <v>1</v>
+      </c>
+      <c r="O34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="5"/>
+      <c r="B35" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" s="2">
+        <v>1</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G35" s="2">
+        <v>0</v>
+      </c>
+      <c r="H35" s="2">
+        <v>0</v>
+      </c>
+      <c r="I35" s="2">
+        <v>0</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="K35" s="2">
+        <v>0</v>
+      </c>
+      <c r="L35" s="2">
+        <v>0</v>
+      </c>
+      <c r="M35" t="s">
+        <v>22</v>
+      </c>
+      <c r="N35" s="2">
+        <v>1</v>
+      </c>
+      <c r="O35" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E36" s="2">
+        <v>2</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G36" s="2">
+        <v>0</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K36" s="2">
+        <v>0</v>
+      </c>
+      <c r="L36" s="2">
+        <v>0</v>
+      </c>
+      <c r="M36" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N36" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O36" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" s="5"/>
+      <c r="B37" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E32" s="2">
+      <c r="C37" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E37" s="2">
         <v>2</v>
       </c>
-      <c r="F32" s="1">
+      <c r="F37" s="1">
         <v>2</v>
       </c>
-      <c r="G32" s="2">
-        <v>1</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I32" t="s">
+      <c r="G37" s="2">
+        <v>1</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I37" t="s">
+        <v>102</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K37" s="2">
+        <v>0</v>
+      </c>
+      <c r="L37" s="2">
+        <v>0</v>
+      </c>
+      <c r="M37" s="4">
+        <v>2</v>
+      </c>
+      <c r="N37" t="s">
         <v>103</v>
       </c>
-      <c r="J32" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K32" s="2">
-        <v>0</v>
-      </c>
-      <c r="L32" s="2">
-        <v>0</v>
-      </c>
-      <c r="M32" s="4">
-        <v>2</v>
-      </c>
-      <c r="N32" t="s">
-        <v>104</v>
-      </c>
-      <c r="O32" t="s">
+      <c r="O37" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:A16"/>
-    <mergeCell ref="A17:A30"/>
-    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A17:A35"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>